<commit_message>
2 runs of dcamp-1m
</commit_message>
<xml_diff>
--- a/analysis/baseline.xlsx
+++ b/analysis/baseline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33520" windowHeight="20140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Chart (Split)" sheetId="2" r:id="rId1"/>
@@ -429,6 +429,42 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Baseline (</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="1" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>dCAMP</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> Off)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -933,11 +969,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2091624216"/>
-        <c:axId val="2091529304"/>
+        <c:axId val="2104376920"/>
+        <c:axId val="2104380056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2091624216"/>
+        <c:axId val="2104376920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,7 +982,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091529304"/>
+        <c:crossAx val="2104380056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -954,7 +990,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091529304"/>
+        <c:axId val="2104380056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -965,7 +1001,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091624216"/>
+        <c:crossAx val="2104376920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1040,6 +1076,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>25th Fibonacci</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'PHP Avg'!$A$2:$A$19</c:f>
@@ -1170,6 +1209,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>5MB Download</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'PHP Avg'!$A$2:$A$19</c:f>
@@ -1307,11 +1349,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2050150152"/>
-        <c:axId val="2050145304"/>
+        <c:axId val="2103788536"/>
+        <c:axId val="2103783048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2050150152"/>
+        <c:axId val="2103788536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,7 +1381,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2050145304"/>
+        <c:crossAx val="2103783048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1347,7 +1389,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2050145304"/>
+        <c:axId val="2103783048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1399,7 +1441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2050150152"/>
+        <c:crossAx val="2103788536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -1426,7 +1468,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -1437,7 +1479,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>